<commit_message>
Perfil jugador, historial y config
</commit_message>
<xml_diff>
--- a/asdasdasd.xlsx
+++ b/asdasdasd.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="104">
   <si>
     <t>Juampi</t>
   </si>
@@ -193,9 +193,6 @@
     <t>user</t>
   </si>
   <si>
-    <t>user_goals</t>
-  </si>
-  <si>
     <t>user_pydmchs</t>
   </si>
   <si>
@@ -232,21 +229,9 @@
     <t>match_id</t>
   </si>
   <si>
-    <t>user_cal</t>
-  </si>
-  <si>
-    <t>FLOAT(2,2)</t>
-  </si>
-  <si>
-    <t>calification</t>
-  </si>
-  <si>
     <t>INT(255)</t>
   </si>
   <si>
-    <t>match_hist</t>
-  </si>
-  <si>
     <t>match_hist_id</t>
   </si>
   <si>
@@ -313,9 +298,6 @@
     <t>VARCHAR(8)</t>
   </si>
   <si>
-    <t>jugado|pendiente</t>
-  </si>
-  <si>
     <t>user_username</t>
   </si>
   <si>
@@ -350,6 +332,36 @@
   </si>
   <si>
     <t>matchs</t>
+  </si>
+  <si>
+    <t>match_det</t>
+  </si>
+  <si>
+    <t>pendiente | confirmado | jugado</t>
+  </si>
+  <si>
+    <t>crear -&gt;</t>
+  </si>
+  <si>
+    <t>pendiente</t>
+  </si>
+  <si>
+    <t>confirmado</t>
+  </si>
+  <si>
+    <t>10 jugadores -&gt;</t>
+  </si>
+  <si>
+    <t>cargar result -&gt;</t>
+  </si>
+  <si>
+    <t>jugado</t>
+  </si>
+  <si>
+    <t>user_wonmatches</t>
+  </si>
+  <si>
+    <t>user_lostmatches</t>
   </si>
 </sst>
 </file>
@@ -1002,7 +1014,7 @@
         <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -1010,7 +1022,7 @@
         <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -1018,10 +1030,10 @@
         <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E5" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
@@ -1029,7 +1041,7 @@
         <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
@@ -1045,7 +1057,7 @@
         <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
@@ -1055,10 +1067,10 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E11" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
@@ -1068,7 +1080,7 @@
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1079,20 +1091,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="6"/>
+    <col min="4" max="4" width="15.85546875" style="6" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.42578125" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" style="6"/>
     <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
@@ -1105,39 +1117,39 @@
         <v>46</v>
       </c>
       <c r="E1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="H1" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="K1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
         <v>43</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>63</v>
-      </c>
       <c r="H2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="K2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1148,90 +1160,90 @@
         <v>44</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" t="s">
         <v>63</v>
       </c>
-      <c r="E3" t="s">
-        <v>68</v>
-      </c>
       <c r="F3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="H3" s="7" t="s">
+      <c r="J3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="K3" s="7" t="s">
         <v>74</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
         <v>51</v>
       </c>
-      <c r="B4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" t="s">
-        <v>52</v>
-      </c>
       <c r="D4" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F4" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="I4" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F6" s="7"/>
       <c r="H6" s="7"/>
@@ -1239,87 +1251,108 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" t="s">
-        <v>49</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B12" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D16" s="9" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G16" s="9"/>
       <c r="J16" s="9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D17" s="6" t="s">
-        <v>73</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D20" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D21" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D22" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>